<commit_message>
Final graphs and stuff
</commit_message>
<xml_diff>
--- a/experimentTimes.xlsx
+++ b/experimentTimes.xlsx
@@ -9,16 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Optimality" sheetId="2" r:id="rId2"/>
+    <sheet name="Time Table" sheetId="3" r:id="rId2"/>
+    <sheet name="Optimality" sheetId="2" r:id="rId3"/>
+    <sheet name="Optimality Averages" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="8" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>Time</t>
   </si>
@@ -126,12 +128,21 @@
   <si>
     <t>FINAL</t>
   </si>
+  <si>
+    <t>Percent of Preferences Fulfilled</t>
+  </si>
+  <si>
+    <t>Percentage of Preferences Fulfilled</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -146,6 +157,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -163,12 +198,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -176,8 +303,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -288,7 +424,7 @@
             <c:numRef>
               <c:f>Sheet1!$I$12:$I$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.0644333333333333</c:v>
@@ -577,7 +713,7 @@
             <c:numRef>
               <c:f>Sheet1!$L$12:$L$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.0644333333333333</c:v>
@@ -891,7 +1027,7 @@
             <c:numRef>
               <c:f>Sheet1!$I$12:$I$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.0644333333333333</c:v>
@@ -966,7 +1102,7 @@
             <c:numRef>
               <c:f>Sheet1!$L$12:$L$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.0644333333333333</c:v>
@@ -1184,6 +1320,1228 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Students vs. </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percent of Preferences Fulfilled</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Optimality!$A$1:$A$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="150"/>
+                <c:pt idx="0">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Optimality!$B$1:$B$150</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="150"/>
+                <c:pt idx="0">
+                  <c:v>0.92975</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.933</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93475</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.933</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93475</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9325</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9345</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.93525</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93325</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.93625</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.93425</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.93025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.93225</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.933</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9295</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.93275</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.935</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9325</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.9295</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.9325</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.92975</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.92825</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.933</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.9305</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.93425</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.93225</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.915375</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.914</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.91425</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.913125</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.911875</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.9155</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.91275</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.91325</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.91575</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.907625</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.915</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.91325</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.915125</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.9145</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.912</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.903875</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.9115</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.912125</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.915375</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.916</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.912375</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.913375</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.915875</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.91575</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.916125</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.91475</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.91475</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.915375</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.914625</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.91425</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.8215</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.8821875</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.8980625</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.900375</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.89875</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.90075</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.8991875</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.8993125</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.90075</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.8724375</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.813625</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.8979375</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.8979375</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.8975</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.903125</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.89925</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.889375</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.8969375</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.901375</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.89825</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.898125</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.8901875</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.900125</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.896875</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.89925</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.900125</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.898875</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.8946875</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.8991875</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.90125</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.826</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.88859375</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.87165625</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.88834375</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.88840625</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.8515</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.83740625</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.89109375</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.76940625</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.8893125</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.8281875</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.891125</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.82590625</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.8885625</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.88940625</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.85784375</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.880875</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.76728125</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.8781875</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.86375</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.7798125</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.84859375</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.89025</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.87215625</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.882</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.717625</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.87540625</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.83215625</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.88971875</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.632578125</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.635421875</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.711640625</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.8069375</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.80009375</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.626640625</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.87459375</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.63790625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.7499375</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.834078125</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.74971875</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.820625</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.710609375</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.858921875</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.775390625</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.84771875</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.88265625</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.803625</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.806796875</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.8441875</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.756984375</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.776875</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.832125</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.79046875</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.851</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.571796875</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.808390625</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.79359375</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.8004375</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.669859375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1985445024"/>
+        <c:axId val="-2004404368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1985445024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2004404368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2004404368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1985445024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1265,6 +2623,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2852,6 +4250,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2916,15 +4830,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2939,6 +4853,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4332,24 +6281,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC372"/>
+  <dimension ref="A1:AF372"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="V336" workbookViewId="0">
-      <selection activeCell="AD346" sqref="AD346"/>
+    <sheetView showRuler="0" topLeftCell="S350" workbookViewId="0">
+      <selection activeCell="AC343" sqref="AC343:AC372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.83203125" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10.83203125" style="4"/>
+    <col min="32" max="32" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4392,8 +6342,14 @@
       <c r="AA1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>8.6999999999999994E-2</v>
       </c>
@@ -4434,8 +6390,15 @@
         <f>AA2/AB2</f>
         <v>0.92974999999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE2">
+        <v>1000</v>
+      </c>
+      <c r="AF2" s="11">
+        <f>AVERAGE(AC2:AC31)</f>
+        <v>0.93246666666666644</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6.7000000000000004E-2</v>
       </c>
@@ -4476,8 +6439,15 @@
         <f t="shared" ref="AC3:AC66" si="0">AA3/AB3</f>
         <v>0.93300000000000005</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE3">
+        <v>2000</v>
+      </c>
+      <c r="AF3" s="11">
+        <f>AVERAGE(AC33:AC62)</f>
+        <v>0.91365000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6.3E-2</v>
       </c>
@@ -4518,8 +6488,15 @@
         <f t="shared" si="0"/>
         <v>0.93</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE4">
+        <v>4000</v>
+      </c>
+      <c r="AF4" s="11">
+        <f>AVERAGE(AC64:AC93)</f>
+        <v>0.8915770833333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6.2E-2</v>
       </c>
@@ -4560,8 +6537,15 @@
         <f t="shared" si="0"/>
         <v>0.93625000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE5">
+        <v>8000</v>
+      </c>
+      <c r="AF5" s="11">
+        <f>AVERAGE(AC188:AC217)</f>
+        <v>0.85451874999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -4602,8 +6586,15 @@
         <f t="shared" si="0"/>
         <v>0.93474999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE6">
+        <v>16000</v>
+      </c>
+      <c r="AF6" s="11">
+        <f>AVERAGE(AC219:AC248)</f>
+        <v>0.76872031250000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6.3E-2</v>
       </c>
@@ -4632,8 +6623,15 @@
         <f t="shared" si="0"/>
         <v>0.93</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE7">
+        <v>32000</v>
+      </c>
+      <c r="AF7" s="11">
+        <f>AVERAGE(AC343:AC372)</f>
+        <v>0.50734479166666679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -4663,7 +6661,7 @@
         <v>0.93125000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6.3E-2</v>
       </c>
@@ -4693,7 +6691,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -4726,7 +6724,7 @@
         <v>0.93474999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6.7000000000000004E-2</v>
       </c>
@@ -4739,16 +6737,16 @@
       <c r="E11">
         <v>100</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="10" t="s">
         <v>29</v>
       </c>
       <c r="X11">
@@ -4768,7 +6766,7 @@
         <v>0.9325</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6.3E-2</v>
       </c>
@@ -4781,17 +6779,17 @@
       <c r="E12">
         <v>100</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <v>1000</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="6">
         <f>AVERAGE(A2:A31)</f>
         <v>6.4433333333333329E-2</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="5">
         <v>100</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="6">
         <f>AVERAGE(D2:D31)</f>
         <v>6.4433333333333329E-2</v>
       </c>
@@ -4815,7 +6813,7 @@
         <v>0.9345</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5.8999999999999997E-2</v>
       </c>
@@ -4828,17 +6826,17 @@
       <c r="E13">
         <v>100</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <v>2000</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="6">
         <f>AVERAGE(A32:A61)</f>
         <v>7.8666666666666676E-2</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="5">
         <v>200</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="6">
         <f>AVERAGE(D32:D61)</f>
         <v>7.7600000000000016E-2</v>
       </c>
@@ -4862,7 +6860,7 @@
         <v>0.93525000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6.3E-2</v>
       </c>
@@ -4875,17 +6873,17 @@
       <c r="E14">
         <v>100</v>
       </c>
-      <c r="H14">
-        <v>4000</v>
-      </c>
-      <c r="I14">
+      <c r="H14" s="5">
+        <v>4000</v>
+      </c>
+      <c r="I14" s="6">
         <f>AVERAGE(A62:A91)</f>
         <v>0.11370000000000005</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="5">
         <v>400</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="6">
         <f>AVERAGE(D62:D91)</f>
         <v>0.17363333333333336</v>
       </c>
@@ -4909,7 +6907,7 @@
         <v>0.93325000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -4922,17 +6920,17 @@
       <c r="E15">
         <v>100</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>8000</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="6">
         <f>AVERAGE(A92:A121)</f>
         <v>0.17883333333333334</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="5">
         <v>800</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="6">
         <f>AVERAGE(D92:D121)</f>
         <v>0.4994333333333334</v>
       </c>
@@ -4956,7 +6954,7 @@
         <v>0.93625000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.06</v>
       </c>
@@ -4969,17 +6967,17 @@
       <c r="E16">
         <v>100</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="7">
         <v>1600</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="8">
         <f>AVERAGE(A122:A151)</f>
         <v>0.30863333333333326</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="7">
         <v>1600</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="8">
         <f>AVERAGE(D122:D151)</f>
         <v>1.9911999999999999</v>
       </c>
@@ -12746,14 +14744,1685 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+      <c r="B2">
+        <v>6.4433333333333301E-2</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>6.4433333333333329E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2000</v>
+      </c>
+      <c r="B3">
+        <v>7.8666666666666676E-2</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <v>7.7600000000000016E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4000</v>
+      </c>
+      <c r="B4">
+        <v>0.11370000000000005</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+      <c r="E4">
+        <v>0.17363333333333336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8000</v>
+      </c>
+      <c r="B5">
+        <v>0.17883333333333334</v>
+      </c>
+      <c r="D5">
+        <v>800</v>
+      </c>
+      <c r="E5">
+        <v>0.4994333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>16000</v>
+      </c>
+      <c r="B6">
+        <v>0.30863333333333326</v>
+      </c>
+      <c r="D6">
+        <v>1600</v>
+      </c>
+      <c r="E6">
+        <v>1.9911999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E180"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1000</v>
+      </c>
+      <c r="B1" s="11">
+        <v>0.92974999999999997</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="11">
+        <f>AVERAGE(B1:B30)</f>
+        <v>0.93246666666666644</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.93</v>
+      </c>
+      <c r="D3">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="11">
+        <f>AVERAGE(B31:B60)</f>
+        <v>0.91365000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.93625000000000003</v>
+      </c>
+      <c r="D4">
+        <v>4000</v>
+      </c>
+      <c r="E4" s="11">
+        <f>AVERAGE(B61:B90)</f>
+        <v>0.8915770833333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.93474999999999997</v>
+      </c>
+      <c r="D5">
+        <v>8000</v>
+      </c>
+      <c r="E5" s="11">
+        <f>AVERAGE(B91:B120)</f>
+        <v>0.85451874999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.93</v>
+      </c>
+      <c r="D6">
+        <v>16000</v>
+      </c>
+      <c r="E6" s="11">
+        <f>AVERAGE(B121:B150)</f>
+        <v>0.76872031250000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.93125000000000002</v>
+      </c>
+      <c r="D7">
+        <v>32000</v>
+      </c>
+      <c r="E7" s="11">
+        <f>AVERAGE(B151:B180)</f>
+        <v>0.50734479166666679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0.93474999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1000</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0.9325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0.9345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="11">
+        <v>0.93525000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1000</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0.93325000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1000</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0.93625000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1000</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0.93425000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1000</v>
+      </c>
+      <c r="B16" s="11">
+        <v>0.93025000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1000</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0.93225000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1000</v>
+      </c>
+      <c r="B18" s="11">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1000</v>
+      </c>
+      <c r="B19" s="11">
+        <v>0.92949999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0.93274999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1000</v>
+      </c>
+      <c r="B21" s="11">
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1000</v>
+      </c>
+      <c r="B22" s="11">
+        <v>0.9325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1000</v>
+      </c>
+      <c r="B23" s="11">
+        <v>0.92949999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1000</v>
+      </c>
+      <c r="B24" s="11">
+        <v>0.9325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1000</v>
+      </c>
+      <c r="B25" s="11">
+        <v>0.92974999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1000</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0.92825000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1000</v>
+      </c>
+      <c r="B27" s="11">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1000</v>
+      </c>
+      <c r="B28" s="11">
+        <v>0.93049999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1000</v>
+      </c>
+      <c r="B29" s="11">
+        <v>0.93425000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1000</v>
+      </c>
+      <c r="B30" s="11">
+        <v>0.93225000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2000</v>
+      </c>
+      <c r="B31" s="11">
+        <v>0.91537500000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2000</v>
+      </c>
+      <c r="B32" s="11">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2000</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0.91425000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2000</v>
+      </c>
+      <c r="B34" s="11">
+        <v>0.91312499999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2000</v>
+      </c>
+      <c r="B35" s="11">
+        <v>0.91187499999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2000</v>
+      </c>
+      <c r="B36" s="11">
+        <v>0.91549999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2000</v>
+      </c>
+      <c r="B37" s="11">
+        <v>0.91274999999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2000</v>
+      </c>
+      <c r="B38" s="11">
+        <v>0.91325000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2000</v>
+      </c>
+      <c r="B39" s="11">
+        <v>0.91574999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2000</v>
+      </c>
+      <c r="B40" s="11">
+        <v>0.90762500000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2000</v>
+      </c>
+      <c r="B41" s="11">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2000</v>
+      </c>
+      <c r="B42" s="11">
+        <v>0.91325000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2000</v>
+      </c>
+      <c r="B43" s="11">
+        <v>0.91512499999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2000</v>
+      </c>
+      <c r="B44" s="11">
+        <v>0.91449999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2000</v>
+      </c>
+      <c r="B45" s="11">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2000</v>
+      </c>
+      <c r="B46" s="11">
+        <v>0.90387499999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2000</v>
+      </c>
+      <c r="B47" s="11">
+        <v>0.91149999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2000</v>
+      </c>
+      <c r="B48" s="11">
+        <v>0.91212499999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2000</v>
+      </c>
+      <c r="B49" s="11">
+        <v>0.91537500000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2000</v>
+      </c>
+      <c r="B50" s="11">
+        <v>0.91600000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2000</v>
+      </c>
+      <c r="B51" s="11">
+        <v>0.91237500000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2000</v>
+      </c>
+      <c r="B52" s="11">
+        <v>0.91337500000000005</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2000</v>
+      </c>
+      <c r="B53" s="11">
+        <v>0.91587499999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2000</v>
+      </c>
+      <c r="B54" s="11">
+        <v>0.91574999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2000</v>
+      </c>
+      <c r="B55" s="11">
+        <v>0.91612499999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2000</v>
+      </c>
+      <c r="B56" s="11">
+        <v>0.91474999999999995</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2000</v>
+      </c>
+      <c r="B57" s="11">
+        <v>0.91474999999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2000</v>
+      </c>
+      <c r="B58" s="11">
+        <v>0.91537500000000005</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2000</v>
+      </c>
+      <c r="B59" s="11">
+        <v>0.91462500000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2000</v>
+      </c>
+      <c r="B60" s="11">
+        <v>0.91425000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>4000</v>
+      </c>
+      <c r="B61" s="11">
+        <v>0.82150000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>4000</v>
+      </c>
+      <c r="B62" s="11">
+        <v>0.88218750000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>4000</v>
+      </c>
+      <c r="B63" s="11">
+        <v>0.89806249999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>4000</v>
+      </c>
+      <c r="B64" s="11">
+        <v>0.90037500000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>4000</v>
+      </c>
+      <c r="B65" s="11">
+        <v>0.89875000000000005</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>4000</v>
+      </c>
+      <c r="B66" s="11">
+        <v>0.90075000000000005</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>4000</v>
+      </c>
+      <c r="B67" s="11">
+        <v>0.89918750000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>4000</v>
+      </c>
+      <c r="B68" s="11">
+        <v>0.89931249999999996</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>4000</v>
+      </c>
+      <c r="B69" s="11">
+        <v>0.90075000000000005</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>4000</v>
+      </c>
+      <c r="B70" s="11">
+        <v>0.87243749999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>4000</v>
+      </c>
+      <c r="B71" s="11">
+        <v>0.81362500000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>4000</v>
+      </c>
+      <c r="B72" s="11">
+        <v>0.89793750000000006</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>4000</v>
+      </c>
+      <c r="B73" s="11">
+        <v>0.89793750000000006</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>4000</v>
+      </c>
+      <c r="B74" s="11">
+        <v>0.89749999999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>4000</v>
+      </c>
+      <c r="B75" s="11">
+        <v>0.90312499999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>4000</v>
+      </c>
+      <c r="B76" s="11">
+        <v>0.89924999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>4000</v>
+      </c>
+      <c r="B77" s="11">
+        <v>0.88937500000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>4000</v>
+      </c>
+      <c r="B78" s="11">
+        <v>0.89693750000000005</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>4000</v>
+      </c>
+      <c r="B79" s="11">
+        <v>0.90137500000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>4000</v>
+      </c>
+      <c r="B80" s="11">
+        <v>0.89824999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>4000</v>
+      </c>
+      <c r="B81" s="11">
+        <v>0.89812499999999995</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>4000</v>
+      </c>
+      <c r="B82" s="11">
+        <v>0.89018750000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>4000</v>
+      </c>
+      <c r="B83" s="11">
+        <v>0.90012499999999995</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>4000</v>
+      </c>
+      <c r="B84" s="11">
+        <v>0.89687499999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>4000</v>
+      </c>
+      <c r="B85" s="11">
+        <v>0.89924999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>4000</v>
+      </c>
+      <c r="B86" s="11">
+        <v>0.90012499999999995</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>4000</v>
+      </c>
+      <c r="B87" s="11">
+        <v>0.89887499999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>4000</v>
+      </c>
+      <c r="B88" s="11">
+        <v>0.89468749999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>4000</v>
+      </c>
+      <c r="B89" s="11">
+        <v>0.89918750000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>4000</v>
+      </c>
+      <c r="B90" s="11">
+        <v>0.90125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>8000</v>
+      </c>
+      <c r="B91" s="11">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>8000</v>
+      </c>
+      <c r="B92" s="11">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>8000</v>
+      </c>
+      <c r="B93" s="11">
+        <v>0.88859374999999996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>8000</v>
+      </c>
+      <c r="B94" s="11">
+        <v>0.87165625000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>8000</v>
+      </c>
+      <c r="B95" s="11">
+        <v>0.88834374999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>8000</v>
+      </c>
+      <c r="B96" s="11">
+        <v>0.88840624999999995</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>8000</v>
+      </c>
+      <c r="B97" s="11">
+        <v>0.85150000000000003</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>8000</v>
+      </c>
+      <c r="B98" s="11">
+        <v>0.83740625000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>8000</v>
+      </c>
+      <c r="B99" s="11">
+        <v>0.89109375000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>8000</v>
+      </c>
+      <c r="B100" s="11">
+        <v>0.76940624999999996</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>8000</v>
+      </c>
+      <c r="B101" s="11">
+        <v>0.88931249999999995</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>8000</v>
+      </c>
+      <c r="B102" s="11">
+        <v>0.82818749999999997</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>8000</v>
+      </c>
+      <c r="B103" s="11">
+        <v>0.89112499999999994</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>8000</v>
+      </c>
+      <c r="B104" s="11">
+        <v>0.82590624999999995</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>8000</v>
+      </c>
+      <c r="B105" s="11">
+        <v>0.88856250000000003</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>8000</v>
+      </c>
+      <c r="B106" s="11">
+        <v>0.88940624999999995</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>8000</v>
+      </c>
+      <c r="B107" s="11">
+        <v>0.85784375000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>8000</v>
+      </c>
+      <c r="B108" s="11">
+        <v>0.88087499999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>8000</v>
+      </c>
+      <c r="B109" s="11">
+        <v>0.76728125000000003</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>8000</v>
+      </c>
+      <c r="B110" s="11">
+        <v>0.87818750000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>8000</v>
+      </c>
+      <c r="B111" s="11">
+        <v>0.86375000000000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>8000</v>
+      </c>
+      <c r="B112" s="11">
+        <v>0.77981250000000002</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>8000</v>
+      </c>
+      <c r="B113" s="11">
+        <v>0.84859375000000004</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>8000</v>
+      </c>
+      <c r="B114" s="11">
+        <v>0.89024999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>8000</v>
+      </c>
+      <c r="B115" s="11">
+        <v>0.87215624999999997</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>8000</v>
+      </c>
+      <c r="B116" s="11">
+        <v>0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>8000</v>
+      </c>
+      <c r="B117" s="11">
+        <v>0.71762499999999996</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>8000</v>
+      </c>
+      <c r="B118" s="11">
+        <v>0.87540625000000005</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>8000</v>
+      </c>
+      <c r="B119" s="11">
+        <v>0.83215625000000004</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>8000</v>
+      </c>
+      <c r="B120" s="11">
+        <v>0.88971875</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>16000</v>
+      </c>
+      <c r="B121" s="4">
+        <v>0.63257812499999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>16000</v>
+      </c>
+      <c r="B122" s="4">
+        <v>0.63542187500000002</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>16000</v>
+      </c>
+      <c r="B123" s="4">
+        <v>0.71164062500000003</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>16000</v>
+      </c>
+      <c r="B124" s="4">
+        <v>0.80693749999999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>16000</v>
+      </c>
+      <c r="B125" s="4">
+        <v>0.80009375000000005</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>16000</v>
+      </c>
+      <c r="B126" s="4">
+        <v>0.62664062499999995</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>16000</v>
+      </c>
+      <c r="B127" s="4">
+        <v>0.87459374999999995</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>16000</v>
+      </c>
+      <c r="B128" s="4">
+        <v>0.63790625000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>16000</v>
+      </c>
+      <c r="B129" s="4">
+        <v>0.74993750000000003</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>16000</v>
+      </c>
+      <c r="B130" s="4">
+        <v>0.834078125</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>16000</v>
+      </c>
+      <c r="B131" s="4">
+        <v>0.74971874999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>16000</v>
+      </c>
+      <c r="B132" s="4">
+        <v>0.82062500000000005</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>16000</v>
+      </c>
+      <c r="B133" s="4">
+        <v>0.71060937499999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>16000</v>
+      </c>
+      <c r="B134" s="4">
+        <v>0.85892187499999995</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>16000</v>
+      </c>
+      <c r="B135" s="4">
+        <v>0.775390625</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>16000</v>
+      </c>
+      <c r="B136" s="4">
+        <v>0.84771874999999997</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>16000</v>
+      </c>
+      <c r="B137" s="4">
+        <v>0.88265625000000003</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>16000</v>
+      </c>
+      <c r="B138" s="4">
+        <v>0.80362500000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>16000</v>
+      </c>
+      <c r="B139" s="4">
+        <v>0.80679687499999997</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>16000</v>
+      </c>
+      <c r="B140" s="4">
+        <v>0.84418749999999998</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>16000</v>
+      </c>
+      <c r="B141" s="4">
+        <v>0.75698437500000004</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>16000</v>
+      </c>
+      <c r="B142" s="4">
+        <v>0.77687499999999998</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>16000</v>
+      </c>
+      <c r="B143" s="4">
+        <v>0.832125</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>16000</v>
+      </c>
+      <c r="B144" s="4">
+        <v>0.79046875000000005</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>16000</v>
+      </c>
+      <c r="B145" s="4">
+        <v>0.85099999999999998</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>16000</v>
+      </c>
+      <c r="B146" s="4">
+        <v>0.57179687499999998</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>16000</v>
+      </c>
+      <c r="B147" s="4">
+        <v>0.80839062500000003</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>16000</v>
+      </c>
+      <c r="B148" s="4">
+        <v>0.79359374999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>16000</v>
+      </c>
+      <c r="B149" s="4">
+        <v>0.80043750000000002</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>16000</v>
+      </c>
+      <c r="B150" s="4">
+        <v>0.66985937500000003</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>32000</v>
+      </c>
+      <c r="B151" s="11">
+        <v>0.64521093750000003</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>32000</v>
+      </c>
+      <c r="B152" s="11">
+        <v>0.55853906249999996</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>32000</v>
+      </c>
+      <c r="B153" s="11">
+        <v>0.40412500000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>32000</v>
+      </c>
+      <c r="B154" s="11">
+        <v>0.45807031250000002</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>32000</v>
+      </c>
+      <c r="B155" s="11">
+        <v>0.40252343750000003</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>32000</v>
+      </c>
+      <c r="B156" s="11">
+        <v>0.51407812500000005</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>32000</v>
+      </c>
+      <c r="B157" s="11">
+        <v>0.59159375000000003</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>32000</v>
+      </c>
+      <c r="B158" s="11">
+        <v>0.58363281249999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>32000</v>
+      </c>
+      <c r="B159" s="11">
+        <v>0.49794531250000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>32000</v>
+      </c>
+      <c r="B160" s="11">
+        <v>0.39896874999999998</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>32000</v>
+      </c>
+      <c r="B161" s="11">
+        <v>0.51014062500000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>32000</v>
+      </c>
+      <c r="B162" s="11">
+        <v>0.57271093750000002</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>32000</v>
+      </c>
+      <c r="B163" s="11">
+        <v>0.50830468750000002</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>32000</v>
+      </c>
+      <c r="B164" s="11">
+        <v>0.62214843750000004</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>32000</v>
+      </c>
+      <c r="B165" s="11">
+        <v>0.42232031250000002</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>32000</v>
+      </c>
+      <c r="B166" s="11">
+        <v>0.50939062499999999</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>32000</v>
+      </c>
+      <c r="B167" s="11">
+        <v>0.42794531250000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>32000</v>
+      </c>
+      <c r="B168" s="11">
+        <v>0.55200000000000005</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>32000</v>
+      </c>
+      <c r="B169" s="11">
+        <v>0.36062499999999997</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>32000</v>
+      </c>
+      <c r="B170" s="11">
+        <v>0.53676562500000002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>32000</v>
+      </c>
+      <c r="B171" s="11">
+        <v>0.3788125</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>32000</v>
+      </c>
+      <c r="B172" s="11">
+        <v>0.49156250000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>32000</v>
+      </c>
+      <c r="B173" s="11">
+        <v>0.52095312500000002</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>32000</v>
+      </c>
+      <c r="B174" s="11">
+        <v>0.46735937500000002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>32000</v>
+      </c>
+      <c r="B175" s="11">
+        <v>0.4964765625</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>32000</v>
+      </c>
+      <c r="B176" s="11">
+        <v>0.58357812499999995</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>32000</v>
+      </c>
+      <c r="B177" s="11">
+        <v>0.47068749999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>32000</v>
+      </c>
+      <c r="B178" s="11">
+        <v>0.57549218749999997</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>32000</v>
+      </c>
+      <c r="B179" s="11">
+        <v>0.50749999999999995</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>32000</v>
+      </c>
+      <c r="B180" s="11">
+        <v>0.65088281250000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.93246666666666644</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2000</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.91365000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4000</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.8915770833333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8000</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.85451874999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>16000</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.76872031250000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>32000</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.50734479166666679</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
including files to be tested
</commit_message>
<xml_diff>
--- a/experimentTimes.xlsx
+++ b/experimentTimes.xlsx
@@ -4871,10 +4871,10 @@
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>